<commit_message>
revised plot type determination to include fenced plots
</commit_message>
<xml_diff>
--- a/Data/data_submission/new_site_info/NutNet-new-site-info_v2_LBB.xlsx
+++ b/Data/data_submission/new_site_info/NutNet-new-site-info_v2_LBB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/NutNet_LBK/Data/data_submission/new_site_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9ADD5D-4420-A745-A3D2-7FC6F2394204}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0922752E-4A4E-CB4C-88A9-4E358FAAE440}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="19400" windowHeight="16620" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16480" yWindow="3700" windowWidth="19400" windowHeight="16620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general-info" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="89">
   <si>
     <t>site_name</t>
   </si>
@@ -299,6 +299,15 @@
   </si>
   <si>
     <t>SW</t>
+  </si>
+  <si>
+    <t>not core plot</t>
+  </si>
+  <si>
+    <t>core control</t>
+  </si>
+  <si>
+    <t>Fence</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1218,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1683,10 +1692,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1736,7 +1745,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D43"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2571,6 +2580,9 @@
       <c r="H2" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="K2" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -2586,16 +2598,16 @@
         <v>82</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2612,7 +2624,7 @@
         <v>83</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>59</v>
@@ -2638,10 +2650,10 @@
         <v>83</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>62</v>
@@ -2664,7 +2676,7 @@
         <v>83</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>81</v>
@@ -2701,6 +2713,9 @@
       <c r="H7" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="K7" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
@@ -2727,6 +2742,9 @@
       <c r="H8" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="K8" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -2742,16 +2760,19 @@
         <v>83</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>59</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2771,7 +2792,7 @@
         <v>61</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>59</v>
@@ -2805,6 +2826,9 @@
       <c r="H11" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="K11" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
@@ -2820,10 +2844,10 @@
         <v>82</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>59</v>
@@ -2846,7 +2870,7 @@
         <v>85</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>59</v>
@@ -2855,7 +2879,7 @@
         <v>59</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2875,10 +2899,10 @@
         <v>59</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>59</v>
@@ -2933,10 +2957,10 @@
         <v>59</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>79</v>
       </c>
@@ -2950,10 +2974,10 @@
         <v>85</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>59</v>
@@ -2962,7 +2986,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>79</v>
       </c>
@@ -2982,13 +3006,13 @@
         <v>59</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>79</v>
       </c>
@@ -3002,10 +3026,10 @@
         <v>83</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>59</v>
@@ -3014,7 +3038,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>79</v>
       </c>
@@ -3039,8 +3063,11 @@
       <c r="H20" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K20" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>79</v>
       </c>
@@ -3060,13 +3087,13 @@
         <v>59</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>79</v>
       </c>
@@ -3080,7 +3107,7 @@
         <v>84</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>81</v>
@@ -3092,7 +3119,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>79</v>
       </c>
@@ -3117,8 +3144,11 @@
       <c r="H23" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K23" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>79</v>
       </c>
@@ -3135,16 +3165,16 @@
         <v>59</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>79</v>
       </c>
@@ -3164,13 +3194,13 @@
         <v>81</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>79</v>
       </c>
@@ -3195,8 +3225,11 @@
       <c r="H26" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K26" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>79</v>
       </c>
@@ -3221,8 +3254,11 @@
       <c r="H27" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K27" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>79</v>
       </c>
@@ -3236,7 +3272,7 @@
         <v>85</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>81</v>
@@ -3248,7 +3284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>79</v>
       </c>
@@ -3262,19 +3298,22 @@
         <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K29" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>79</v>
       </c>
@@ -3291,7 +3330,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>62</v>
@@ -3300,7 +3339,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>79</v>
       </c>
@@ -3314,10 +3353,10 @@
         <v>83</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>59</v>
@@ -3326,7 +3365,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>79</v>
       </c>
@@ -3351,8 +3390,11 @@
       <c r="H32" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K32" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>79</v>
       </c>
@@ -3366,7 +3408,7 @@
         <v>84</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>59</v>
@@ -3378,7 +3420,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>79</v>
       </c>
@@ -3392,19 +3434,19 @@
         <v>82</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>79</v>
       </c>
@@ -3418,7 +3460,7 @@
         <v>83</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>81</v>
@@ -3427,10 +3469,10 @@
         <v>62</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>79</v>
       </c>
@@ -3447,16 +3489,16 @@
         <v>59</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>59</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>79</v>
       </c>
@@ -3470,19 +3512,19 @@
         <v>85</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>79</v>
       </c>
@@ -3496,19 +3538,22 @@
         <v>85</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K38" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
@@ -3533,8 +3578,11 @@
       <c r="H39" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K39" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>79</v>
       </c>
@@ -3551,16 +3599,16 @@
         <v>59</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>79</v>
       </c>
@@ -3585,8 +3633,11 @@
       <c r="H41" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K41" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>79</v>
       </c>
@@ -3611,8 +3662,11 @@
       <c r="H42" s="11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="K42" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>79</v>
       </c>
@@ -3626,13 +3680,13 @@
         <v>84</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>59</v>
@@ -3649,7 +3703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5DCDFC-9BE7-914D-B92D-B9914F7A4DD0}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>